<commit_message>
fix XLSX file to use int instead of excel bool type
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -10745,7 +10745,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -10806,6 +10806,13 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -10972,7 +10979,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11149,23 +11156,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11186,6 +11181,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11269,28 +11268,28 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="55.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="56.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="38.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="14.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="15.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="37.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="70.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="189.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="37.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="35.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="65.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="181.78"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="18" style="3" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1023" style="3" width="11.54"/>
   </cols>
@@ -35278,18 +35277,18 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="40" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="40" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="49.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="40" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="40" width="80.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="86.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="40" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="40" width="141.49"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="8" style="40" width="11.52"/>
   </cols>
   <sheetData>
@@ -35418,18 +35417,18 @@
   </sheetPr>
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="40" width="5.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="32.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="80.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="32.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="41" width="80.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="40" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="40" width="37.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="8" style="40" width="11.52"/>
   </cols>
@@ -35441,7 +35440,7 @@
       <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="44" t="s">
         <v>3498</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -35450,7 +35449,7 @@
       <c r="E1" s="7" t="s">
         <v>3512</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="9" t="s">
         <v>3513</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -35477,7 +35476,7 @@
       <c r="B2" s="16" t="s">
         <v>3515</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="45" t="s">
         <v>3516</v>
       </c>
       <c r="D2" s="16" t="n">
@@ -35486,8 +35485,7 @@
       <c r="E2" s="16" t="s">
         <v>3517</v>
       </c>
-      <c r="F2" s="47" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F2" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="16" t="s">
@@ -35508,7 +35506,7 @@
       <c r="B3" s="16" t="s">
         <v>3520</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="45" t="s">
         <v>3516</v>
       </c>
       <c r="D3" s="16" t="n">
@@ -35517,8 +35515,7 @@
       <c r="E3" s="16" t="s">
         <v>3517</v>
       </c>
-      <c r="F3" s="47" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F3" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="16" t="s">
@@ -35533,7 +35530,7 @@
       <c r="B4" s="16" t="s">
         <v>3522</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="45" t="s">
         <v>3516</v>
       </c>
       <c r="D4" s="16" t="n">
@@ -35542,8 +35539,7 @@
       <c r="E4" s="16" t="s">
         <v>3517</v>
       </c>
-      <c r="F4" s="47" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F4" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="16" t="s">
@@ -35558,7 +35554,7 @@
       <c r="B5" s="16" t="s">
         <v>3524</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="45" t="s">
         <v>3516</v>
       </c>
       <c r="D5" s="16" t="n">
@@ -35567,8 +35563,7 @@
       <c r="E5" s="16" t="s">
         <v>3517</v>
       </c>
-      <c r="F5" s="47" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F5" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="16" t="s">
@@ -35583,7 +35578,7 @@
       <c r="B6" s="16" t="s">
         <v>3526</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="45" t="s">
         <v>3516</v>
       </c>
       <c r="D6" s="16" t="n">
@@ -35592,8 +35587,7 @@
       <c r="E6" s="16" t="s">
         <v>3517</v>
       </c>
-      <c r="F6" s="47" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F6" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="16" t="s">
@@ -35608,7 +35602,7 @@
       <c r="B7" s="16" t="s">
         <v>3528</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="45" t="s">
         <v>3516</v>
       </c>
       <c r="D7" s="16" t="n">
@@ -35617,8 +35611,7 @@
       <c r="E7" s="16" t="s">
         <v>3517</v>
       </c>
-      <c r="F7" s="47" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F7" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="16" t="s">
@@ -35633,7 +35626,7 @@
       <c r="B8" s="16" t="s">
         <v>3530</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="45" t="s">
         <v>3516</v>
       </c>
       <c r="D8" s="16" t="n">
@@ -35642,8 +35635,7 @@
       <c r="E8" s="16" t="s">
         <v>3517</v>
       </c>
-      <c r="F8" s="47" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F8" s="16" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="16" t="s">
@@ -35652,83 +35644,63 @@
       <c r="AMJ8" s="43"/>
     </row>
     <row r="9" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="48"/>
       <c r="AMJ9" s="43"/>
     </row>
     <row r="10" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="48"/>
       <c r="AMJ10" s="43"/>
     </row>
     <row r="11" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="48"/>
       <c r="AMJ11" s="43"/>
     </row>
     <row r="12" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="48"/>
       <c r="AMJ12" s="43"/>
     </row>
     <row r="13" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="48"/>
       <c r="AMJ13" s="43"/>
     </row>
     <row r="14" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="48"/>
       <c r="AMJ14" s="43"/>
     </row>
     <row r="15" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="48"/>
       <c r="AMJ15" s="43"/>
     </row>
     <row r="16" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="48"/>
       <c r="AMJ16" s="43"/>
     </row>
     <row r="17" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="48"/>
       <c r="AMJ17" s="43"/>
     </row>
     <row r="18" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="48"/>
       <c r="AMJ18" s="43"/>
     </row>
     <row r="19" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="48"/>
       <c r="AMJ19" s="43"/>
     </row>
     <row r="20" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="48"/>
       <c r="AMJ20" s="43"/>
     </row>
     <row r="21" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="48"/>
       <c r="AMJ21" s="43"/>
     </row>
     <row r="22" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="48"/>
       <c r="AMJ22" s="43"/>
     </row>
     <row r="23" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="48"/>
       <c r="AMJ23" s="43"/>
     </row>
     <row r="24" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="48"/>
       <c r="AMJ24" s="43"/>
     </row>
     <row r="25" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="48"/>
       <c r="AMJ25" s="43"/>
     </row>
     <row r="26" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="48"/>
       <c r="AMJ26" s="43"/>
     </row>
     <row r="27" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="48"/>
       <c r="AMJ27" s="43"/>
     </row>
     <row r="28" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="48"/>
       <c r="AMJ28" s="43"/>
     </row>
   </sheetData>
@@ -35758,19 +35730,31 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="19.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="3" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="49" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="3" width="15.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="19.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="46" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="14.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="54.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="56.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="15.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="18" style="3" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="50" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="47" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -35780,19 +35764,19 @@
       <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="48" t="s">
         <v>3531</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="48" t="s">
         <v>3532</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="48" t="s">
         <v>3533</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="48" t="s">
         <v>3534</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="49" t="s">
         <v>3535</v>
       </c>
       <c r="H1" s="7" t="s">
@@ -35801,33 +35785,33 @@
       <c r="I1" s="7" t="s">
         <v>3537</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="50" t="s">
         <v>3538</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="50" t="s">
         <v>3539</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="50" t="s">
         <v>3540</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="50" t="s">
         <v>3541</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="N1" s="50" t="s">
         <v>3542</v>
       </c>
-      <c r="O1" s="53" t="s">
+      <c r="O1" s="50" t="s">
         <v>3543</v>
       </c>
-      <c r="P1" s="53" t="s">
+      <c r="P1" s="50" t="s">
         <v>3544</v>
       </c>
-      <c r="Q1" s="53" t="s">
+      <c r="Q1" s="50" t="s">
         <v>3545</v>
       </c>
-      <c r="AMH1" s="50"/>
-      <c r="AMI1" s="50"/>
-      <c r="AMJ1" s="50"/>
+      <c r="AMH1" s="47"/>
+      <c r="AMI1" s="47"/>
+      <c r="AMJ1" s="47"/>
     </row>
     <row r="2" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -35848,8 +35832,7 @@
       <c r="F2" s="16" t="s">
         <v>3550</v>
       </c>
-      <c r="G2" s="47" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="G2" s="16" t="n">
         <v>1</v>
       </c>
       <c r="H2" s="16" t="n">
@@ -35881,8 +35864,7 @@
       <c r="F3" s="16" t="s">
         <v>3550</v>
       </c>
-      <c r="G3" s="47" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="G3" s="16" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="16" t="n">
@@ -35914,8 +35896,7 @@
       <c r="F4" s="16" t="s">
         <v>3550</v>
       </c>
-      <c r="G4" s="47" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="G4" s="16" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="16" t="n">
@@ -35947,8 +35928,7 @@
       <c r="F5" s="16" t="s">
         <v>3550</v>
       </c>
-      <c r="G5" s="47" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="G5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="16" t="n">
@@ -35980,8 +35960,7 @@
       <c r="F6" s="16" t="s">
         <v>3550</v>
       </c>
-      <c r="G6" s="47" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="G6" s="16" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="16" t="n">
@@ -36001,17 +35980,17 @@
       <c r="B7" s="16" t="s">
         <v>3561</v>
       </c>
-      <c r="G7" s="47"/>
+      <c r="G7" s="51"/>
       <c r="H7" s="16" t="n">
         <v>10</v>
       </c>
       <c r="I7" s="16" t="n">
         <v>20</v>
       </c>
-      <c r="K7" s="46" t="s">
+      <c r="K7" s="45" t="s">
         <v>3562</v>
       </c>
-      <c r="L7" s="46" t="s">
+      <c r="L7" s="45" t="s">
         <v>3563</v>
       </c>
       <c r="M7" s="16" t="s">
@@ -36034,37 +36013,37 @@
       <c r="AMJ7" s="21"/>
     </row>
     <row r="8" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="47"/>
+      <c r="G8" s="51"/>
       <c r="AMH8" s="21"/>
       <c r="AMI8" s="21"/>
       <c r="AMJ8" s="21"/>
     </row>
     <row r="9" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G9" s="47"/>
+      <c r="G9" s="51"/>
       <c r="AMH9" s="21"/>
       <c r="AMI9" s="21"/>
       <c r="AMJ9" s="21"/>
     </row>
     <row r="10" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G10" s="47"/>
+      <c r="G10" s="51"/>
       <c r="AMH10" s="21"/>
       <c r="AMI10" s="21"/>
       <c r="AMJ10" s="21"/>
     </row>
     <row r="11" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="47"/>
+      <c r="G11" s="51"/>
       <c r="AMH11" s="21"/>
       <c r="AMI11" s="21"/>
       <c r="AMJ11" s="21"/>
     </row>
     <row r="12" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="47"/>
+      <c r="G12" s="51"/>
       <c r="AMH12" s="21"/>
       <c r="AMI12" s="21"/>
       <c r="AMJ12" s="21"/>
     </row>
     <row r="13" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G13" s="47"/>
+      <c r="G13" s="51"/>
       <c r="AMH13" s="21"/>
       <c r="AMI13" s="21"/>
       <c r="AMJ13" s="21"/>

</xml_diff>